<commit_message>
Added DataProviders for Register and Search and modified excel test data
</commit_message>
<xml_diff>
--- a/src/main/resources/com/demoapp/qa/testData/DemoAppTestData.xlsx
+++ b/src/main/resources/com/demoapp/qa/testData/DemoAppTestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600" firstSheet="5" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="ValidLogin" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,11 @@
     <sheet name="InvalidEmailAndValidPassLogin" sheetId="3" r:id="rId3"/>
     <sheet name="ValidEmailAndInvalidPassLogin" sheetId="4" r:id="rId4"/>
     <sheet name="BlankCredentialsLogin" sheetId="5" r:id="rId5"/>
+    <sheet name="MandateFieldsReg" sheetId="6" r:id="rId6"/>
+    <sheet name="AllFieldsReg" sheetId="7" r:id="rId7"/>
+    <sheet name="ExistingEmailReg" sheetId="8" r:id="rId8"/>
+    <sheet name="ValidProductSearch" sheetId="11" r:id="rId9"/>
+    <sheet name="InvalidProductSearch" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="16">
   <si>
     <t>Email</t>
   </si>
@@ -49,6 +54,33 @@
   </si>
   <si>
     <t>Warning: No match for E-Mail Address and/or Password.</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Telephone</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Valid Product Name</t>
+  </si>
+  <si>
+    <t>Baking Soda</t>
+  </si>
+  <si>
+    <t>Invalid Product Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HP </t>
   </si>
 </sst>
 </file>
@@ -458,6 +490,34 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
@@ -552,7 +612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -619,4 +679,186 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1">
+        <v>8333412132</v>
+      </c>
+      <c r="D2" s="1">
+        <v>12345</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1">
+        <v>8333412132</v>
+      </c>
+      <c r="D2" s="1">
+        <v>12345</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>8333412132</v>
+      </c>
+      <c r="E2" s="1">
+        <v>12345</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>